<commit_message>
Update XL files with translation edits
</commit_message>
<xml_diff>
--- a/inputs/fr/demo_demo_input.xlsx
+++ b/inputs/fr/demo_demo_input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aimee.altermatt\Documents\GitHub\Nutrition\inputs\fr\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4B2F9B4B-EF62-49D2-93D6-901A42E1201E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C653898F-305D-423C-AC81-3B78BBEB5E73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="1140" windowWidth="14400" windowHeight="7360" tabRatio="885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -510,7 +510,7 @@
     <t>Année finale</t>
   </si>
   <si>
-    <t>Données sur la population</t>
+    <t>Données démographiques</t>
   </si>
   <si>
     <t>Population des enfants de moins de 5 ans</t>
@@ -1056,7 +1056,7 @@
     <t>En forme de S (coût marginal décroissant puis croissant)</t>
   </si>
   <si>
-    <t>Efficacité</t>
+    <t>efficacité</t>
   </si>
   <si>
     <t>Retard de croissance</t>
@@ -1146,19 +1146,19 @@
     <t>Anémique</t>
   </si>
   <si>
-    <t xml:space="preserve">Risque relatif des causes du décès par mode d'allaitement maternel </t>
+    <t>Risque relatif des causes du décès par mode d'allaitement maternel</t>
   </si>
   <si>
     <t>Mode d'allaitement maternel</t>
   </si>
   <si>
-    <t xml:space="preserve">Risques relatifs de la diarrhée par mode d'allaitement maternel </t>
+    <t>Risques relatifs de la diarrhée par mode d'allaitement maternel</t>
   </si>
   <si>
     <t>Risque relatif des causes du décès par la distribution du poids-pour-taille (amaigrissement)</t>
   </si>
   <si>
-    <t>Avec retard de croissance précédent (HAZ &lt; -2 dans la tranche d'àge précédente)</t>
+    <t>Compte tenu du retard de croissance antérieur (HAZ &lt; -2 dans la tranche d’âge précédente)</t>
   </si>
   <si>
     <t>Diarrhée (par épisode supplémentaire)</t>
@@ -5191,7 +5191,7 @@
       <c r="A63" s="4"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="J0ExHI3s4jkyFfvkbLmdJsCccteNAQANHaVOdU+bVKcPLtCFpLg3+4Lma7JAdIHcCcasw4/hqQLgI0cs+0vE4w==" saltValue="phXyZBLA+o9ACGo2vXYwvA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="BcHNrpLfM7nfwFuJ56nBD9SekFreI/mU/6zZ3TLUqoPSRnl61RLTtXteRCJoQKoIRJWUp5toocaMt7Q1bjUcXg==" saltValue="2+7KvU1PSpS7lMsL4PCNEA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
 </worksheet>
@@ -5290,7 +5290,7 @@
       <c r="A19" s="48"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="9ihL1YCLP7ZMl6hlTFOyfpdEO/FzNNOY6nmroU1zLrPiABKkPNMUPegdQXpm2a11p6aaxO+4V/8mCYW6KK1h0Q==" saltValue="g0fvXNGZ2gFtdrD9Xloevw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="ZrcZpBKXqEqhkD4wC3YGwHqV8WAaJPIZxVitPdbv7Ahfn5D5qnWJ6OOUg9S+QDqlNjcPxl9p9F/OcoG26YWlJQ==" saltValue="eXyfJ2cmnQRkUj7gWiVp9g==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -5405,7 +5405,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="L6GDoSUFoKFzs2LL+lT4jaqsjL/mx2YvctEOLx1ukQE3gVEG/x/mIJUnE8JZai5uEAZD3q/1l7dFR9yd3URB2A==" saltValue="bNQXR6PGqnvQBhwf90BRPA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="SZenVMSSUiDaRc0ObwgG6XL7c0CCtt4FSxcTCIKuGhu6mtS8tR2YpjptuCIspKHKXlMJqQlTItGuNt7S7oS5Zw==" saltValue="PvTxfjQ6oaunes608qC/CA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -7121,7 +7121,7 @@
       <c r="B39" s="33"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="yJrZ2yet0l4ltZfNaZfpjryY+cBYhp5nHeCuZ6iNkdICs3xeh4wa1rGC3bX/tK7Vqm8TsES2Gx7/p1ItSTVxPw==" saltValue="ngELuUobDIctXUAn4QHSTw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="wC3WhJriwjxt8T14kBd8nqcmbZnNfhedYSfOD0QEut+rKpkeP9JbXhe7Gmk8cxNScj1GRTHoVZ1DFzH7/dYniA==" saltValue="+MthxhPqON54l9/rQKVzXQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B14:O21">
     <sortCondition ref="B14:B21"/>
   </sortState>
@@ -7272,7 +7272,7 @@
       <c r="C20" s="85"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="gNI+cfC5WkNiY3iuz0jOdaL1gY6q2YWx39J8l98HXOWKhSrp0BNDtmWuOhFT8l7xqEZB9fzMd8ibRY19h4WTzg==" saltValue="j2l0TxVJV0GNKIEDVJLiTQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="sTnOSxlh9KLUcimGUPyUmb7/Q9vsM31I5lzsRHgTC7FaRre2YXLzVfwBrxoTiaUdStsxicxE59FWu+6THpDWdw==" saltValue="M4XWUDc0+PjxqyjkUv54Yw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
@@ -7308,7 +7308,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="kqto8WS3Wo1UXugiYqvpt+SRlI4kguMlzQOQlNsgqeIdUZQhcXmKIE+CvD7HOiwRwDXUor/D0KWfeZHF8plXZA==" saltValue="fRIcZcytZNT63fp5B3C+qg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="KBbLFAo9QuKoPXXBL04m0FbXgWrWVb+V9xNDnCHBpqhItolP8eohDSKzcpN+jBrLFqYUpnIfbsbcCUHVu524DQ==" saltValue="PkSMSBVhjGB4NOziHb5TRQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -7516,7 +7516,7 @@
       <c r="C11" s="36"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="jPTGWNtqhMxXMaW6YKKDlEIlbPAql2Cu+zHd4oSZ8VyyK2qbqAnUfSYH26M/jP0Ho2HfWGT+D/+/k/fh94CIqQ==" saltValue="oIW1V1R/6VELmyARja3KBw==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="gZhlmSGHPEXUilJ07M4WJd74LSNWpVktP92TVQHNsAYQzEvZbUJFWvjXFV+BuHIeSGVqxcJ7eohiwJNzHSDgUA==" saltValue="dK7BN+TI7aESKznhPGXKlA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
@@ -9287,7 +9287,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="KCTd60vzkoofIdr1a2+qat0ZDOKYvPW13fkurjcuCsnvep+Q4xZG8TDb+recmSY+Ek/kZtAQzFo6Ig8Edo1RVQ==" saltValue="Chz2eZpBzYGgG3e7ZtEkYw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="B7O//Gujh4Qr4UBSSWsLqJ60CPIkK5qRudWifcujmQSnh6hrTUQ76C/7SfugIkyuv0QeqWQchXfgk7ffzUABVA==" saltValue="l0s/M45O+iZdBkqu5O4o8A==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -10033,7 +10033,7 @@
       <c r="K38" s="133"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="JXAvslkaUWURPT13sBLs/dON7iUnXtJQ9Rnplurr7QOmFy0thjUsqlAt0ZXIhmTGGYbwEMKlWIJMsI6mD7jiUQ==" saltValue="OxhgvwQGbOQ8MwevG96lyA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="tI92hNUbbehs+KplGGIaUzxPW2S4UYoY5ImWizYT+eTCD8drfMh6gxASOt7l5oIWoFGb0W77oXscBfpZ7MxQBw==" saltValue="w0DejQQBvVf4ew41TeVHgw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -10407,7 +10407,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="SXacT22WZtgFy1JIMMyqbf4tBGJEWf9pufTpVPaxXrfFZKLXZ7XcQE1vvhs4yRVWUzUK0pkVN+RQIZJIhJhO1Q==" saltValue="f9wEHgjWbR5jnZlRG2suLQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="MWBQvZIkdMeNHJP7INYBaKwpHahk8dhqAaLTGCq0ecnERJgO0PKQm1ikZB4iMyE3yM/htSF4JrYACGTXia3EHQ==" saltValue="cBAhJO2Yt2efi1rmAQJgVQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -11528,7 +11528,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="3sU6FcIJI/f5DDxjZXG41nVBKx1gX5wrL3N463uEQscpN/7HWM939OUeepDmyFL0BKdIQzpX/ZE/BVdu1/nY1A==" saltValue="xBYrO9KE5UbcQjB1AQMdDw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="o5CDTHSK+TLhJAiqs8SV2AqTItqn3mY6qhyxVC1EmWchTDIAuBUL9NpJcmCVhURseG5YBDFo2YXylCMV5fvicw==" saltValue="9Z34lGhIteulbQl8a+b0ag==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="15">
     <mergeCell ref="B19:B21"/>
     <mergeCell ref="B2:B4"/>
@@ -12636,7 +12636,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="IvZ7QAE/hamg/WoK5UwRqYbYGwx2l2ZJplB/9UJjKujsySwoR06qUZxMnrh3GiFyyJugyx/g2NQEgPgAGLV8/A==" saltValue="Fb6YihupynY9JmtTCrE07g==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="hAGFWxvf8YUfpcYWTC00AAMAkin1ZOHzWtDWSxCo5PC9wcOnOkn8brprMwU5Z+b59p8iZjuntjD6+HWixijp2A==" saltValue="y6vkIepzzJ98CAYDiKwVRg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <conditionalFormatting sqref="B2:I40">
     <cfRule type="expression" dxfId="0" priority="9">
       <formula>$A2=""</formula>
@@ -13038,7 +13038,7 @@
       <c r="B28" s="40"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="4JwenSzYu49LStpE1gLZwOtMGsqEMX2j74F+CEXLbot1D9gpsQk0t/Ec0PbaNr0DZsMl13wojnatoOgtmtHLpA==" saltValue="gBsUcLbVKtmQd66jcFQYyA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="d6NPMVWOcm0lsfz/SIT9rjITFQU19Nyxd9HBNeT0+49Syf17tPGdPkrvSf437igdvhVnwVQyLkeInG8/Zb7JQg==" saltValue="VQmdG8W65PmA79jqa/LLLg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -15941,7 +15941,7 @@
       <c r="A111" s="40"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="MA3EzEpJHh0yaFP0zI+WrM+x+hPNtx6pNoXXDsqUoC+7pN0IC1F3qcjb1s/o3EaUMwLusRwVb1TJ9nfoCs5Zqw==" saltValue="xPbcEEUBL6MLnQKofuLRCg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="i8mN3ZhyB0Nyaj6k903abhPx4HCgCvCMja3iAUYsWLrm71Y+YaBrjFwz2oMJXwgxODleJOxo3o21HOd6C0asPw==" saltValue="WexCPU1sWkYXt2Mhc9U/Hw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -16250,7 +16250,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="FO6TiQogdO5JpHf4M+bYH6DcOkg17pTJkdABx1tqdgGjANJS98Br3EC8eW5k/qw08IYlk9VJJmAyyqhMu/Quog==" saltValue="ClQqPYRxdo2s2dmC72me4w==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="VMjARlJJax3cxDtxolkhCXTPbMRl9CDq1UxHhFbTH3Sqfaa/lAMdvdTI2EoQAB5qwgGqPeogVKR6cpF4thUa5g==" saltValue="OCPnDgxGMV/gUhDzLZARFw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
@@ -16530,7 +16530,7 @@
       <c r="A20" s="90"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="DTy9+BGKcThlt8PFZeWbSDnwNROA2O7TIehTAGNXMRQfXsqkNFELwy1BXaBUdNmFeGLGBnwqkbU/njsC4RJlLw==" saltValue="hNxQH2Hg0D2ed/hHQrW6Kw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="JspThBlELRPKHJ1KVh2DOEMK4wgz6rqAntWM+nVeqawAxH1UmdhguUvYtc6Yd4v2Qy4rhUsrdF8taBvVUs/KYA==" saltValue="ii9u4bX8w+bKxgub8ptSQA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -17326,7 +17326,7 @@
       <c r="B28" s="43"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="t3bMWFRoDp7g3XmpPbEO7kwWDvOq32r/r8NkvjC3oX96sHagsko9SnEjUUbqq/p1wi5YbELpNxEyoc4MCcyRKg==" saltValue="qimFG0o9IrelI3oktGy8mg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="u+IvWOJX34Vek7R1wBMfac8Wb6Vrv298j+ZxDWSBgCEi7LO8i2wFiugea7cCWGdBTZ1ESmsVX4+x4iOT/yD3cg==" saltValue="2yx7/2zQwLZ34uBBgLF7YQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -17427,7 +17427,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="gdXwEAJfZ4BberSgq9kz3Da3XY5TZ/gnAgOyfzhRIskzVmmdf9BAOsNaB7ekIRtGW4tmbaMert/GN5YIUI24gQ==" saltValue="w7GWq3PYuNptwLh72FYPNg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="MR9Z0ZT9pIEbm4eH4On9z1WeJKEHCCqD0NzqzqA7D3fBzk0PcnOQWe3lQPhQb8dfwQhz1b3LmdnAputHViynCQ==" saltValue="2ZkGISKaJxLSbg5GfAziEA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -18557,7 +18557,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="qF+EnXDI4Z9Mr2EnnvCHtBI5NWOzut6TlYht8oEwwcmdQ1D00blZqMVWkDgjM3LiNeJJYnmc1ZgKXxbmuJBBJA==" saltValue="rx2cbgRUeMKuCuUlToKImg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="R7uuK1Ez0KE90nGEXK3NWLyN0iq4P8giyyxTh8QIO989xOjVszOIw0bhzRdT+8c33/XqluGgIdtr/DCTU8GyZA==" saltValue="33ic6PQHnwj3dJk/Iso2yQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
 </worksheet>
@@ -18734,7 +18734,7 @@
       <c r="H7" s="128"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="2v7GocQwg7lVKT6tpKmOdElguP/1w1LW6iDRKYj+qn1Vd9wAzHXxEGsB72ZddF2BuD3KWjWMNfdu/KKyVMbA+A==" saltValue="2mgyTlbG1pKc1CT/jzA6lg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="q33I46+ainvlxUZ/jDewCVkdA89MBpdP/dr85m6EpHxDFlV8UT5+wMvPG1arhaY+MKoWqrgjIT5nC64NJNAOUg==" saltValue="ww+Tn9IQf6aEdEOE5ul5cQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -19171,7 +19171,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="3jax2JYBzEloiGEvSaLQBapifXu6WvJEVER8yjcK0GQhnRPSN5ITag/icO4pGYnQ6ctDRM1Y+JoMmPrXARSX5Q==" saltValue="L4dI3XKSXmvCk0ZNtZXjRA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="mjSMCGS04fWouObPbPfOmCSDQS4Ly2dAW7Po8grqEwAq+kJzPkT+QGhULnV5yICLz9ND/QumTmT/wjIxpsL47Q==" saltValue="fIChv0KkUDJAfv9W9EwDkQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="69" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -19598,7 +19598,7 @@
       <c r="G17" s="8"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="1wjMS14zhQfNj39i3pGUXyj/VyzDK27WmVBPQyLfotJvgyTgvFPjtus8yBhcBbKRTyIyhjwpPBa3AgZJO20bBw==" saltValue="9nedOfX2MXuibawerKlNfg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="2hYO+aWG3LxkebJaR15+A9FsxFPmaNIS1R0Y/8jl/iefSzZjNxPHBeJES6LoPlzGtQda6ttIMAjw5w4gtHY+3w==" saltValue="Oj1jFAPsHoLMHu2ieIgjJw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
@@ -19735,7 +19735,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="8BpDBQMRb+Rw4SBSBYVhfGD47Yms+D8Q3T/m5fDoHKn0gYbOttN/TT+e+feN2J83vb+gw/2hLrdX7pyWekJuBw==" saltValue="rSAYHKMh41nhbsABGhmohA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="Qi0c2w0ySyoK27uxlajDrijllBG0Sc/wp3aAfokhpdyCba1q3gR675f1zhnNrmjp5lQ7OVAfM6s8rR2jm1iwzQ==" saltValue="I+oBbxi1evvpA/6foWDjIQ==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -20051,7 +20051,7 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="l/GQ1nHSnu1gD/S9wgBI36/mJbGpsMRSBgvq4IfIjzOryhHx3eLZ+eRXR9N8CyhuXm/CDyMMUVgSehmxW0EAfw==" saltValue="8iZsIAAgqbFO6rQfjZQLIQ==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="f3v6CIVjSmpIDg6PWBOcxvjm2suEjVyN1o8XhaWFEJpHynoBL16KNCFw2PxXEyGg/Vb+xk6UPz9zvrkzoZqjdA==" saltValue="2Gtsqdi23iwoA55Mi80l7w==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="193" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -20329,7 +20329,7 @@
       <c r="E21" s="80"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="nseBIhw/321h3D31G7r0kG29LldYqyrhb/Z/BjCHRWUA1FSUjNhuglh1wn8K17Rom0eD057VIOs88FPsVeg/rA==" saltValue="5mRwl8xohWflz8aymip2Sg==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="0VbhM9vM9PYo4cScqUJEBVuuDvsOF+kTig/2/nmr515TvlBFLXi1oJN1oLMf+45M9IHN4iy9NQntw5y2bUkLcg==" saltValue="vjWp6CJPV5X7WnOtB7KgVA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -20393,7 +20393,7 @@
       <c r="D3" s="80"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Ii6hozaMnNg4Grfo/FZLLuFuIa3wsnqPVuPUktscN3UavKJcanXQ+rExzMUSx9+t3/m8DpbL54ykrILSNC8qxA==" saltValue="ugXLFjHpJ0KQMliFdPn5uA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="zt9kuH4/6vFabDm3Nb4VTfMaI06JqaNOCqctc8+/qM4bahPKEuWDDHuqE9AQLx+Te8i81JlQTN6kinwo2D8M8A==" saltValue="y3yixpcuW7Lxepmgy7l//A==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -21071,7 +21071,7 @@
       <c r="F39" s="36"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="E9j8KwNzGT18Tmnia3DqE9y7CLvl/Oa8MinwXbCgJP8lIEtcpFZJjMOvgMN8dDy7LbCcTycKBAkDAOulzu+dtw==" saltValue="/YJUXdmfOc3PZjY64hPncA==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="6P9i6LBVWPXUK6uLLq/zuDFVrxNzXiQUnYm7QdPj6An9L1a7HsjQJc/OJ6YBPrPOQLktADrPco2z47t6+TLRvA==" saltValue="iNw0QL/HtjfHoQTQCZtSyw==" spinCount="100000" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D38">
     <sortCondition ref="A2:A38"/>
   </sortState>

</xml_diff>